<commit_message>
1. bernoulli 2. take out the variance of labor income and unemployment income
</commit_message>
<xml_diff>
--- a/data/age_coefficients_and_var.xlsx
+++ b/data/age_coefficients_and_var.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40640" yWindow="10380" windowWidth="18440" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Coefficients" sheetId="2" r:id="rId1"/>
     <sheet name="Variance" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Table 2 - Variance Decomposition</t>
   </si>
   <si>
-    <t>Panel A - Labor Income Only</t>
-  </si>
-  <si>
     <t>No High School</t>
   </si>
   <si>
@@ -61,6 +58,15 @@
   </si>
   <si>
     <t>b3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Table 2 - Variance Decomposition</t>
+  </si>
+  <si>
+    <t>Labor Income Only</t>
+  </si>
+  <si>
+    <t>Labor Income Plus Unemployment Income</t>
   </si>
 </sst>
 </file>
@@ -111,12 +117,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -152,18 +164,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
@@ -446,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,21 +477,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <f>-2.170042+2.700381</f>
@@ -492,7 +511,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <f>-2.170042+2.700381</f>
@@ -512,22 +531,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <f>-2.170042+2.700381</f>
-        <v>0.53033900000000012</v>
-      </c>
-      <c r="C4">
-        <v>0.16818</v>
-      </c>
-      <c r="D4">
-        <f>-0.0323371/10</f>
-        <v>-3.2337099999999999E-3</v>
-      </c>
-      <c r="E4">
-        <f>0.0019704/100</f>
-        <v>1.9704000000000003E-5</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>-51819.03</v>
+      </c>
+      <c r="C4" s="11">
+        <v>3553.4589999999998</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.93375940000000002</v>
+      </c>
+      <c r="E4" s="11">
+        <v>-0.5499252</v>
       </c>
     </row>
   </sheetData>
@@ -538,10 +554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,50 +566,83 @@
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
       <c r="B4" s="2">
-        <v>0.16900000000000001</v>
+        <v>0.15716233645501712</v>
       </c>
       <c r="C4" s="2">
         <v>0.13711309200802088</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.14499999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="7">
+        <v>0.14387494569938158</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.16911534525287764</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.1374772708486752</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.14525839046333949</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>-3.0000000000000001E-3</v>
       </c>
@@ -603,22 +652,40 @@
       <c r="D5" s="2">
         <v>-1.8E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="3">
+        <v>-2.8999999999999998E-3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>-1.6999999999999999E-3</v>
+      </c>
+      <c r="G5" s="3">
+        <v>-1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>0.38500000000000001</v>
+        <v>0.3391902121229326</v>
       </c>
       <c r="C6" s="2">
-        <v>0.28199999999999997</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.26300000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.23377339455121918</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.22956480566497992</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.38529209698616967</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.28178005607210743</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.26258332011001767</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>-1.8599999999999998E-2</v>
       </c>
@@ -628,11 +695,22 @@
       <c r="D7" s="2">
         <v>-1.12E-2</v>
       </c>
+      <c r="E7" s="6">
+        <v>-1.8200000000000001E-2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>-1.8200000000000001E-2</v>
+      </c>
+      <c r="G7" s="6">
+        <v>-1.0699999999999999E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
confirm CE result still right
</commit_message>
<xml_diff>
--- a/data/age_coefficients_and_var.xlsx
+++ b/data/age_coefficients_and_var.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="21600" yWindow="6860" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Coefficients" sheetId="2" r:id="rId1"/>
@@ -158,11 +158,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -176,18 +178,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
+    <sheetView zoomScale="187" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -533,16 +537,16 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>-51819.03</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>3553.4589999999998</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>0.93375940000000002</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>-0.5499252</v>
       </c>
     </row>
@@ -556,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,31 +576,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
1. add pi and theta into optimization model 2. income process simulation
</commit_message>
<xml_diff>
--- a/data/age_coefficients_and_var.xlsx
+++ b/data/age_coefficients_and_var.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21600" yWindow="6860" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1160" yWindow="1920" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Coefficients" sheetId="2" r:id="rId1"/>
@@ -470,7 +470,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="187" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,19 +498,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>-2.170042+2.700381</f>
-        <v>0.53033900000000012</v>
+        <v>41078.879999999997</v>
       </c>
       <c r="C2">
-        <v>0.16818</v>
+        <v>-2201.5819999999999</v>
       </c>
       <c r="D2">
-        <f>-0.0323371/10</f>
-        <v>-3.2337099999999999E-3</v>
+        <v>78.223410000000001</v>
       </c>
       <c r="E2">
-        <f>0.0019704/100</f>
-        <v>1.9704000000000003E-5</v>
+        <v>-0.78894830000000005</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -518,19 +515,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f>-2.170042+2.700381</f>
-        <v>0.53033900000000012</v>
+        <v>28752.76</v>
       </c>
       <c r="C3">
-        <v>0.16818</v>
+        <v>-917.54660000000001</v>
       </c>
       <c r="D3">
-        <f>-0.0323371/10</f>
-        <v>-3.2337099999999999E-3</v>
+        <v>51.095140000000001</v>
       </c>
       <c r="E3">
-        <f>0.0019704/100</f>
-        <v>1.9704000000000003E-5</v>
+        <v>-0.60892809999999997</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -561,7 +555,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,10 +621,10 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="7">
         <v>0.15716233645501712</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="7">
         <v>0.13711309200802088</v>
       </c>
       <c r="D4" s="7">
@@ -670,10 +664,10 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="7">
         <v>0.3391902121229326</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="7">
         <v>0.23377339455121918</v>
       </c>
       <c r="D6" s="7">

</xml_diff>